<commit_message>
Added Map Layers, cleaned up Characteristics
</commit_message>
<xml_diff>
--- a/src/characteristics/data/Used in Models.xlsx
+++ b/src/characteristics/data/Used in Models.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnwall\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gis\usgs\ss\Applications\StreamStatsNationalServices\src\characteristics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21780" windowHeight="4116"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22935" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="308">
   <si>
     <t>CAT_PPT7100_ANN</t>
   </si>
@@ -939,12 +939,21 @@
   </si>
   <si>
     <t>source location</t>
+  </si>
+  <si>
+    <t>Done?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -976,7 +985,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -999,16 +1008,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1289,20 +1320,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I89"/>
+  <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="92.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="92" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>296</v>
       </c>
@@ -1330,8 +1367,11 @@
       <c r="I1" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J1" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1359,8 +1399,11 @@
       <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J2" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1388,8 +1431,11 @@
       <c r="I3" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J3" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -1417,8 +1463,11 @@
       <c r="I4" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J4" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1446,8 +1495,11 @@
       <c r="I5" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J5" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -1475,8 +1527,11 @@
       <c r="I6" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J6" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -1504,8 +1559,11 @@
       <c r="I7" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J7" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
@@ -1533,8 +1591,11 @@
       <c r="I8" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J8" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
@@ -1562,8 +1623,11 @@
       <c r="I9" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J9" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>48</v>
       </c>
@@ -1591,8 +1655,11 @@
       <c r="I10" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J10" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>53</v>
       </c>
@@ -1620,8 +1687,11 @@
       <c r="I11" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J11" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>56</v>
       </c>
@@ -1649,8 +1719,11 @@
       <c r="I12" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J12" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
@@ -1678,8 +1751,11 @@
       <c r="I13" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J13" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>62</v>
       </c>
@@ -1707,8 +1783,11 @@
       <c r="I14" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J14" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>65</v>
       </c>
@@ -1736,8 +1815,11 @@
       <c r="I15" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J15" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>68</v>
       </c>
@@ -1765,8 +1847,11 @@
       <c r="I16" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J16" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>71</v>
       </c>
@@ -1794,8 +1879,11 @@
       <c r="I17" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J17" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>74</v>
       </c>
@@ -1823,8 +1911,11 @@
       <c r="I18" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J18" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>77</v>
       </c>
@@ -1852,8 +1943,11 @@
       <c r="I19" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J19" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>80</v>
       </c>
@@ -1881,8 +1975,11 @@
       <c r="I20" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J20" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>83</v>
       </c>
@@ -1910,8 +2007,11 @@
       <c r="I21" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J21" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>86</v>
       </c>
@@ -1939,8 +2039,11 @@
       <c r="I22" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J22" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>91</v>
       </c>
@@ -1968,8 +2071,11 @@
       <c r="I23" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J23" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>94</v>
       </c>
@@ -1997,8 +2103,11 @@
       <c r="I24" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J24" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>97</v>
       </c>
@@ -2026,8 +2135,11 @@
       <c r="I25" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J25" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>100</v>
       </c>
@@ -2055,8 +2167,11 @@
       <c r="I26" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J26" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>103</v>
       </c>
@@ -2084,8 +2199,11 @@
       <c r="I27" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J27" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>106</v>
       </c>
@@ -2113,8 +2231,11 @@
       <c r="I28" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J28" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>109</v>
       </c>
@@ -2142,8 +2263,11 @@
       <c r="I29" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J29" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>112</v>
       </c>
@@ -2171,8 +2295,11 @@
       <c r="I30" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J30" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>115</v>
       </c>
@@ -2200,8 +2327,11 @@
       <c r="I31" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J31" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>118</v>
       </c>
@@ -2229,8 +2359,11 @@
       <c r="I32" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J32" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>121</v>
       </c>
@@ -2258,8 +2391,11 @@
       <c r="I33" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J33" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>124</v>
       </c>
@@ -2287,8 +2423,11 @@
       <c r="I34" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J34" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>129</v>
       </c>
@@ -2316,8 +2455,11 @@
       <c r="I35" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J35" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>132</v>
       </c>
@@ -2345,8 +2487,11 @@
       <c r="I36" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J36" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>135</v>
       </c>
@@ -2374,8 +2519,11 @@
       <c r="I37" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J37" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>138</v>
       </c>
@@ -2403,8 +2551,11 @@
       <c r="I38" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J38" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>141</v>
       </c>
@@ -2432,8 +2583,11 @@
       <c r="I39" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J39" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>144</v>
       </c>
@@ -2461,8 +2615,11 @@
       <c r="I40" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J40" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>147</v>
       </c>
@@ -2490,8 +2647,11 @@
       <c r="I41" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J41" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>150</v>
       </c>
@@ -2519,8 +2679,11 @@
       <c r="I42" s="2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J42" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>153</v>
       </c>
@@ -2548,8 +2711,11 @@
       <c r="I43" s="2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J43" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>156</v>
       </c>
@@ -2577,8 +2743,11 @@
       <c r="I44" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J44" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>159</v>
       </c>
@@ -2606,8 +2775,11 @@
       <c r="I45" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J45" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>162</v>
       </c>
@@ -2635,8 +2807,11 @@
       <c r="I46" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J46" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>167</v>
       </c>
@@ -2664,8 +2839,11 @@
       <c r="I47" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J47" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>172</v>
       </c>
@@ -2693,8 +2871,11 @@
       <c r="I48" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J48" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>179</v>
       </c>
@@ -2722,8 +2903,11 @@
       <c r="I49" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J49" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>185</v>
       </c>
@@ -2751,8 +2935,11 @@
       <c r="I50" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J50" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>191</v>
       </c>
@@ -2780,8 +2967,11 @@
       <c r="I51" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J51" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>196</v>
       </c>
@@ -2809,8 +2999,11 @@
       <c r="I52" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J52" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>203</v>
       </c>
@@ -2838,8 +3031,11 @@
       <c r="I53" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J53" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>205</v>
       </c>
@@ -2867,8 +3063,11 @@
       <c r="I54" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J54" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>207</v>
       </c>
@@ -2896,8 +3095,11 @@
       <c r="I55" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J55" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>209</v>
       </c>
@@ -2925,8 +3127,11 @@
       <c r="I56" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J56" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>211</v>
       </c>
@@ -2954,8 +3159,11 @@
       <c r="I57" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J57" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>213</v>
       </c>
@@ -2983,8 +3191,11 @@
       <c r="I58" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J58" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>215</v>
       </c>
@@ -3012,8 +3223,11 @@
       <c r="I59" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J59" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>217</v>
       </c>
@@ -3041,8 +3255,11 @@
       <c r="I60" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J60" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>219</v>
       </c>
@@ -3070,8 +3287,11 @@
       <c r="I61" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J61" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>221</v>
       </c>
@@ -3099,8 +3319,11 @@
       <c r="I62" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J62" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>223</v>
       </c>
@@ -3128,8 +3351,11 @@
       <c r="I63" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J63" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>225</v>
       </c>
@@ -3157,8 +3383,11 @@
       <c r="I64" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J64" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>227</v>
       </c>
@@ -3186,8 +3415,11 @@
       <c r="I65" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J65" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>229</v>
       </c>
@@ -3215,8 +3447,11 @@
       <c r="I66" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J66" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>231</v>
       </c>
@@ -3244,8 +3479,11 @@
       <c r="I67" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J67" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>233</v>
       </c>
@@ -3273,8 +3511,11 @@
       <c r="I68" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J68" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>241</v>
       </c>
@@ -3302,8 +3543,11 @@
       <c r="I69" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J69" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>243</v>
       </c>
@@ -3331,8 +3575,11 @@
       <c r="I70" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J70" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>246</v>
       </c>
@@ -3360,8 +3607,11 @@
       <c r="I71" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J71" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>248</v>
       </c>
@@ -3389,8 +3639,11 @@
       <c r="I72" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J72" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>250</v>
       </c>
@@ -3418,8 +3671,11 @@
       <c r="I73" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J73" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>255</v>
       </c>
@@ -3447,8 +3703,11 @@
       <c r="I74" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J74" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>257</v>
       </c>
@@ -3476,8 +3735,11 @@
       <c r="I75" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J75" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>259</v>
       </c>
@@ -3505,8 +3767,11 @@
       <c r="I76" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J76" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>261</v>
       </c>
@@ -3534,8 +3799,11 @@
       <c r="I77" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J77" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>263</v>
       </c>
@@ -3563,8 +3831,11 @@
       <c r="I78" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J78" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>268</v>
       </c>
@@ -3592,8 +3863,11 @@
       <c r="I79" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J79" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>271</v>
       </c>
@@ -3621,8 +3895,11 @@
       <c r="I80" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J80" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>273</v>
       </c>
@@ -3650,8 +3927,11 @@
       <c r="I81" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J81" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>275</v>
       </c>
@@ -3679,8 +3959,11 @@
       <c r="I82" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J82" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>277</v>
       </c>
@@ -3708,8 +3991,11 @@
       <c r="I83" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J83" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>279</v>
       </c>
@@ -3737,8 +4023,11 @@
       <c r="I84" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J84" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>282</v>
       </c>
@@ -3766,8 +4055,11 @@
       <c r="I85" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J85" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>285</v>
       </c>
@@ -3795,8 +4087,11 @@
       <c r="I86" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J86" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>288</v>
       </c>
@@ -3824,8 +4119,11 @@
       <c r="I87" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J87" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>292</v>
       </c>
@@ -3853,8 +4151,11 @@
       <c r="I88" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J88" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>294</v>
       </c>
@@ -3881,6 +4182,9 @@
       </c>
       <c r="I89" s="2" t="s">
         <v>254</v>
+      </c>
+      <c r="J89" s="3" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>